<commit_message>
add clean file and format excel
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>CL</t>
   </si>
@@ -26,10 +26,10 @@
     <t>MRP</t>
   </si>
   <si>
+    <t>#</t>
+  </si>
+  <si>
     <t>MRP Q.</t>
-  </si>
-  <si>
-    <t>#</t>
   </si>
   <si>
     <t>Q. scar.</t>
@@ -125,20 +125,20 @@
 Lavorazione Linea 5: euro/kg. 0.264 x 4050.0 = 1069.2
 Costi materie prime:
 Lavoration LAH/004045:
- - A1224: EUR 0.77 x q. 2800.0 = 2156.0
- - A0102: EUR 0.62 x q. 240.0 = 148.8
- - A0404: EUR 0.92 x q. 420.0 = 386.4
- - A0405: EUR 0.325 x q. 420.0 = 136.5
- - A0601: EUR 1.09 x q. 32.0 = 34.88
- - A2035: EUR 4.4 x q. 8.0 = 35.2
-Totale materie prime: 2897.78
+ - A1224: EUR 12100.0 x q. 2800.0 = 33880000.0
+ - A0102: EUR 3150.0 x q. 240.0 = 756000.0
+ - A0404: EUR 4900.0 x q. 420.0 = 2058000.0
+ - A0405: EUR 2400.0 x q. 420.0 = 1008000.0
+ - A0601: EUR 900.0 x q. 32.0 = 28800.0
+ - A2035: EUR 180.0 x q. 8.0 = 1440.0
+Totale materie prime: 37732240.0
 Costi imballi e pallet:
  - Imballo [LAH/004045] B6003: EUR 0.405 x q. 162 = 65.61
- - Pallet [LAH/004045] B6107: EUR 10.7 x q. 4 = 42.8 
-Totale imballi: 3006.19
+ - Pallet [LAH/004045] B6107: EUR 360.0 x q. 4 = 1440.0 
+Totale imballi: 37733745.61
 Peso materie prime: 3920.0
 Costo totale:
-EUR 4075.39 : q. 4050.0 = EUR/unit 1.0062691358 (carico)
+EUR 37734814.81 : q. 4050.0 = EUR/unit 9317.23822469 (carico)
 </t>
   </si>
   <si>
@@ -187,21 +187,21 @@
 Lavorazione Linea 4: euro/kg. 0.264 x 6050.0 = 1597.2
 Costi materie prime:
 Lavoration LAH/004047:
- - A1004: EUR 0.645 x q. 969.0 = 625.005
- - A1216: EUR 0.68 x q. 969.0 = 658.92
- - A0600: EUR 0.98 x q. 229.5 = 224.91
- - A3004: EUR 2.4 x q. 102.0 = 244.8
- - A0402: EUR 0.88 x q. 17.85 = 15.708
- - A0404: EUR 0.92 x q. 384.03 = 353.3076
- - A0403: EUR 0.31 x q. 2428.62 = 752.8722
-Totale materie prime: 2875.5228
+ - A1004: EUR 30900.0 x q. 969.0 = 29942100.0
+ - A1216: EUR 15540.0 x q. 969.0 = 15058260.0
+ - A0600: EUR 3000.0 x q. 229.5 = 688500.0
+ - A3004: EUR 880.0 x q. 102.0 = 89760.0
+ - A0402: EUR 3000.0 x q. 17.85 = 53550.0
+ - A0404: EUR 4900.0 x q. 384.03 = 1881747.0
+ - A0403: EUR 8000.0 x q. 2428.62 = 19428960.0
+Totale materie prime: 67142877.0
 Costi imballi e pallet:
  - Imballo [LAH/004047] B6003: EUR 0.405 x q. 242 = 98.01
- - Pallet [LAH/004047] B6107: EUR 10.7 x q. 6 = 64.2 
-Totale imballi: 3037.7328
+ - Pallet [LAH/004047] B6107: EUR 360.0 x q. 6 = 2160.0 
+Totale imballi: 67145135.01
 Peso materie prime: 5100.0
 Costo totale:
-EUR 4634.9328 : q. 6050.0 = EUR/unit 0.766104595041 (carico)
+EUR 67146732.21 : q. 6050.0 = EUR/unit 11098.6334231 (carico)
 </t>
   </si>
 </sst>
@@ -209,7 +209,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,16 +217,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -234,12 +253,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,43 +581,43 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -607,13 +647,13 @@
         <v>34</v>
       </c>
       <c r="J2">
-        <v>0.98546</v>
+        <v>4050</v>
       </c>
       <c r="K2">
-        <v>1.006269135802469</v>
+        <v>9317.238224691358</v>
       </c>
       <c r="L2">
-        <v>-0.02080913580246913</v>
+        <v>-5267.238224691358</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -645,16 +685,13 @@
         <v>48</v>
       </c>
       <c r="J3">
-        <v>0.81349</v>
+        <v>1000</v>
       </c>
       <c r="K3">
-        <v>0.7661045950413224</v>
+        <v>11098.6334231405</v>
       </c>
       <c r="L3">
-        <v>0.0473854049586776</v>
-      </c>
-      <c r="M3" t="s">
-        <v>47</v>
+        <v>-10098.6334231405</v>
       </c>
     </row>
   </sheetData>
@@ -671,247 +708,262 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="B1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1">
-        <v>0.77</v>
+      <c r="E1" s="2">
+        <v>12100</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="B2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2">
-        <v>0.62</v>
+      <c r="E2" s="2">
+        <v>3150</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="B3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3">
-        <v>0.92</v>
+      <c r="E3" s="2">
+        <v>4900</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="B4" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4">
-        <v>0.325</v>
+      <c r="E4" s="2">
+        <v>2400</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="B5" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5">
-        <v>1.09</v>
+      <c r="E5" s="2">
+        <v>900</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6">
-        <v>4.4</v>
+      <c r="E6" s="2">
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.405</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="B8" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8">
-        <v>10.7</v>
+      <c r="E8" s="2">
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E9">
-        <v>0.645</v>
+      <c r="E9" s="2">
+        <v>30900</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E10">
-        <v>0.68</v>
+      <c r="E10" s="2">
+        <v>15540</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="B11" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E11">
-        <v>0.98</v>
+      <c r="E11" s="2">
+        <v>3000</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="B12" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E12">
-        <v>2.4</v>
+      <c r="E12" s="2">
+        <v>880</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="B13" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E13">
-        <v>0.88</v>
+      <c r="E13" s="2">
+        <v>3000</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="B14" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E14">
-        <v>0.92</v>
+      <c r="E14" s="2">
+        <v>4900</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="B15" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E15">
-        <v>0.31</v>
+      <c r="E15" s="2">
+        <v>8000</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>0.405</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E17">
-        <v>10.7</v>
+      <c r="E17" s="2">
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generic bugfix (fast message)
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>CL</t>
   </si>
@@ -125,20 +125,20 @@
 Lavorazione Linea 5: euro/kg. 0.264 x 4050.0 = 1069.2
 Costi materie prime:
 Lavoration LAH/004045:
- - A1224: EUR 12100.0 x q. 2800.0 = 33880000.0
- - A0102: EUR 3150.0 x q. 240.0 = 756000.0
- - A0404: EUR 4900.0 x q. 420.0 = 2058000.0
- - A0405: EUR 2400.0 x q. 420.0 = 1008000.0
- - A0601: EUR 900.0 x q. 32.0 = 28800.0
- - A2035: EUR 180.0 x q. 8.0 = 1440.0
-Totale materie prime: 37732240.0
+ - A1224: EUR 0.77 x q. 2800.0 = 2156.0
+ - A0102: EUR 0.62 x q. 240.0 = 148.8
+ - A0404: EUR 0.92 x q. 420.0 = 386.4
+ - A0405: EUR 0.325 x q. 420.0 = 136.5
+ - A0601: EUR 1.09 x q. 32.0 = 34.88
+ - A2035: EUR 4.4 x q. 8.0 = 35.2
+Totale materie prime: 2897.78
 Costi imballi e pallet:
  - Imballo [LAH/004045] B6003: EUR 0.405 x q. 162 = 65.61
- - Pallet [LAH/004045] B6107: EUR 360.0 x q. 4 = 1440.0 
-Totale imballi: 37733745.61
+ - Pallet [LAH/004045] B6107: EUR 10.7 x q. 4 = 42.8 
+Totale imballi: 3006.19
 Peso materie prime: 3920.0
 Costo totale:
-EUR 37734814.81 : q. 4050.0 = EUR/unit 9317.23822469 (carico)
+EUR 4075.39 : q. 4050.0 = EUR/unit 1.0062691358 (carico)
 </t>
   </si>
   <si>
@@ -187,21 +187,21 @@
 Lavorazione Linea 4: euro/kg. 0.264 x 6050.0 = 1597.2
 Costi materie prime:
 Lavoration LAH/004047:
- - A1004: EUR 30900.0 x q. 969.0 = 29942100.0
- - A1216: EUR 15540.0 x q. 969.0 = 15058260.0
- - A0600: EUR 3000.0 x q. 229.5 = 688500.0
- - A3004: EUR 880.0 x q. 102.0 = 89760.0
- - A0402: EUR 3000.0 x q. 17.85 = 53550.0
- - A0404: EUR 4900.0 x q. 384.03 = 1881747.0
- - A0403: EUR 8000.0 x q. 2428.62 = 19428960.0
-Totale materie prime: 67142877.0
+ - A1004: EUR 0.645 x q. 969.0 = 625.005
+ - A1216: EUR 0.68 x q. 969.0 = 658.92
+ - A0600: EUR 0.98 x q. 229.5 = 224.91
+ - A3004: EUR 2.4 x q. 102.0 = 244.8
+ - A0402: EUR 0.88 x q. 17.85 = 15.708
+ - A0404: EUR 0.92 x q. 384.03 = 353.3076
+ - A0403: EUR 0.31 x q. 2428.62 = 752.8722
+Totale materie prime: 2875.5228
 Costi imballi e pallet:
  - Imballo [LAH/004047] B6003: EUR 0.405 x q. 242 = 98.01
- - Pallet [LAH/004047] B6107: EUR 360.0 x q. 6 = 2160.0 
-Totale imballi: 67145135.01
+ - Pallet [LAH/004047] B6107: EUR 10.7 x q. 6 = 64.2 
+Totale imballi: 3037.7328
 Peso materie prime: 5100.0
 Costo totale:
-EUR 67146732.21 : q. 6050.0 = EUR/unit 11098.6334231 (carico)
+EUR 4634.9328 : q. 6050.0 = EUR/unit 0.766104595041 (carico)
 </t>
   </si>
 </sst>
@@ -221,13 +221,13 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -579,6 +579,21 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
@@ -622,76 +637,81 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>4050</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>4050</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>3920</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J2">
-        <v>4050</v>
-      </c>
-      <c r="K2">
-        <v>9317.238224691358</v>
-      </c>
-      <c r="L2">
-        <v>-5267.238224691358</v>
-      </c>
+      <c r="J2" s="2">
+        <v>0.98546</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.006269135802469</v>
+      </c>
+      <c r="L2" s="2">
+        <v>-0.02080913580246913</v>
+      </c>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>6050</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>6050</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>5100</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J3">
-        <v>1000</v>
-      </c>
-      <c r="K3">
-        <v>11098.6334231405</v>
-      </c>
-      <c r="L3">
-        <v>-10098.6334231405</v>
+      <c r="J3" s="2">
+        <v>0.81349</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.7661045950413224</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.0473854049586776</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +739,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="2">
-        <v>12100</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -734,7 +754,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="2">
-        <v>3150</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -749,7 +769,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="2">
-        <v>4900</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -764,7 +784,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="2">
-        <v>2400</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -779,7 +799,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="2">
-        <v>900</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -794,7 +814,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="2">
-        <v>180</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -826,7 +846,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="2">
-        <v>360</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -841,7 +861,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="2">
-        <v>30900</v>
+        <v>0.645</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -856,7 +876,7 @@
         <v>37</v>
       </c>
       <c r="E10" s="2">
-        <v>15540</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -871,7 +891,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="2">
-        <v>3000</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -886,7 +906,7 @@
         <v>40</v>
       </c>
       <c r="E12" s="2">
-        <v>880</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -901,7 +921,7 @@
         <v>42</v>
       </c>
       <c r="E13" s="2">
-        <v>3000</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -916,7 +936,7 @@
         <v>19</v>
       </c>
       <c r="E14" s="2">
-        <v>4900</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -931,7 +951,7 @@
         <v>17</v>
       </c>
       <c r="E15" s="2">
-        <v>8000</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -963,7 +983,7 @@
         <v>17</v>
       </c>
       <c r="E17" s="2">
-        <v>360</v>
+        <v>10.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>